<commit_message>
Lots of small changes including better optimization of binary operations
</commit_message>
<xml_diff>
--- a/models/models/data/tox_test.xlsx
+++ b/models/models/data/tox_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Mobius2\models\models\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA997F76-F71D-4953-98FE-2408C4201EBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4638510-60FC-470B-83C8-78235E5A9141}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{D0E19786-DA9A-4277-8346-8F1041FBB6FD}"/>
   </bookViews>
@@ -33,10 +33,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>spline_interpolate</t>
+    <t>Contaminant conc in precip</t>
   </si>
   <si>
-    <t>Contaminant conc in precip</t>
+    <t>linear_interpolate</t>
   </si>
 </sst>
 </file>
@@ -396,7 +396,7 @@
   <dimension ref="A1:C10958"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,13 +406,13 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -460,7 +460,7 @@
         <v>38353</v>
       </c>
       <c r="B8" s="2">
-        <v>0.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -468,7 +468,7 @@
         <v>40179</v>
       </c>
       <c r="B9" s="2">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -476,7 +476,7 @@
         <v>42005</v>
       </c>
       <c r="B10" s="2">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -484,7 +484,7 @@
         <v>43831</v>
       </c>
       <c r="B11" s="2">
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>